<commit_message>
December 2019 employment and earnings data update
</commit_message>
<xml_diff>
--- a/static/data/source/unemployment_rate.xlsx
+++ b/static/data/source/unemployment_rate.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\EHuffer\AppData\Local\Box\Box Edit\Documents\tL7TceG7nkeoPTq_b1ea5w==\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\EHuffer\AppData\Local\Box\Box Edit\Documents\tA0VW6Yfj0K6Fcos_Fe9Vw==\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -723,10 +723,10 @@
   <dimension ref="A1:TO56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="SY5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="SW5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="TJ14" sqref="TJ14"/>
+      <selection pane="bottomRight" activeCell="TK15" sqref="TK15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3817,7 +3817,7 @@
         <v>4.7</v>
       </c>
       <c r="SA5" s="4">
-        <v>4.7</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="SB5" s="4">
         <v>4.4000000000000004</v>
@@ -3859,7 +3859,7 @@
         <v>4</v>
       </c>
       <c r="SO5" s="4">
-        <v>3.9</v>
+        <v>4</v>
       </c>
       <c r="SP5" s="4">
         <v>3.8</v>
@@ -3868,7 +3868,7 @@
         <v>4</v>
       </c>
       <c r="SR5" s="4">
-        <v>3.9</v>
+        <v>3.8</v>
       </c>
       <c r="SS5" s="4">
         <v>3.8</v>
@@ -3916,6 +3916,9 @@
         <v>3.6</v>
       </c>
       <c r="TH5" s="8">
+        <v>3.5</v>
+      </c>
+      <c r="TI5" s="8">
         <v>3.5</v>
       </c>
     </row>
@@ -5504,6 +5507,9 @@
       <c r="TH6" s="8">
         <v>2.7</v>
       </c>
+      <c r="TI6" s="8">
+        <v>2.7</v>
+      </c>
     </row>
     <row r="7" spans="1:529" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
@@ -7090,6 +7096,9 @@
       <c r="TH7" s="8">
         <v>6.1</v>
       </c>
+      <c r="TI7" s="8">
+        <v>6.1</v>
+      </c>
     </row>
     <row r="8" spans="1:529" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
@@ -8676,6 +8685,9 @@
       <c r="TH8" s="8">
         <v>4.7</v>
       </c>
+      <c r="TI8" s="8">
+        <v>4.5999999999999996</v>
+      </c>
     </row>
     <row r="9" spans="1:529" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
@@ -10262,6 +10274,9 @@
       <c r="TH9" s="8">
         <v>3.6</v>
       </c>
+      <c r="TI9" s="8">
+        <v>3.6</v>
+      </c>
     </row>
     <row r="10" spans="1:529" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
@@ -11848,6 +11863,9 @@
       <c r="TH10" s="8">
         <v>3.9</v>
       </c>
+      <c r="TI10" s="8">
+        <v>3.9</v>
+      </c>
     </row>
     <row r="11" spans="1:529" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
@@ -13434,6 +13452,9 @@
       <c r="TH11" s="8">
         <v>2.6</v>
       </c>
+      <c r="TI11" s="8">
+        <v>2.5</v>
+      </c>
     </row>
     <row r="12" spans="1:529" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
@@ -15020,6 +15041,9 @@
       <c r="TH12" s="8">
         <v>3.7</v>
       </c>
+      <c r="TI12" s="8">
+        <v>3.7</v>
+      </c>
     </row>
     <row r="13" spans="1:529" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
@@ -16606,6 +16630,9 @@
       <c r="TH13" s="8">
         <v>3.8</v>
       </c>
+      <c r="TI13" s="8">
+        <v>3.9</v>
+      </c>
     </row>
     <row r="14" spans="1:529" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
@@ -18192,6 +18219,9 @@
       <c r="TH14" s="8">
         <v>5.3</v>
       </c>
+      <c r="TI14" s="8">
+        <v>5.3</v>
+      </c>
     </row>
     <row r="15" spans="1:529" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
@@ -19778,6 +19808,9 @@
       <c r="TH15" s="8">
         <v>3.1</v>
       </c>
+      <c r="TI15" s="8">
+        <v>3</v>
+      </c>
     </row>
     <row r="16" spans="1:529" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
@@ -21364,8 +21397,11 @@
       <c r="TH16" s="8">
         <v>3.3</v>
       </c>
+      <c r="TI16" s="8">
+        <v>3.2</v>
+      </c>
     </row>
-    <row r="17" spans="1:528" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:529" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>13</v>
       </c>
@@ -22950,8 +22986,11 @@
       <c r="TH17" s="8">
         <v>2.6</v>
       </c>
+      <c r="TI17" s="8">
+        <v>2.6</v>
+      </c>
     </row>
-    <row r="18" spans="1:528" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:529" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>14</v>
       </c>
@@ -24536,8 +24575,11 @@
       <c r="TH18" s="8">
         <v>2.9</v>
       </c>
+      <c r="TI18" s="8">
+        <v>2.9</v>
+      </c>
     </row>
-    <row r="19" spans="1:528" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:529" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>15</v>
       </c>
@@ -26122,8 +26164,11 @@
       <c r="TH19" s="8">
         <v>3.8</v>
       </c>
+      <c r="TI19" s="8">
+        <v>3.7</v>
+      </c>
     </row>
-    <row r="20" spans="1:528" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:529" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>16</v>
       </c>
@@ -27708,8 +27753,11 @@
       <c r="TH20" s="8">
         <v>3.2</v>
       </c>
+      <c r="TI20" s="8">
+        <v>3.2</v>
+      </c>
     </row>
-    <row r="21" spans="1:528" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:529" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>17</v>
       </c>
@@ -29294,8 +29342,11 @@
       <c r="TH21" s="8">
         <v>2.6</v>
       </c>
+      <c r="TI21" s="8">
+        <v>2.7</v>
+      </c>
     </row>
-    <row r="22" spans="1:528" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:529" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>18</v>
       </c>
@@ -30880,8 +30931,11 @@
       <c r="TH22" s="8">
         <v>3.1</v>
       </c>
+      <c r="TI22" s="8">
+        <v>3.2</v>
+      </c>
     </row>
-    <row r="23" spans="1:528" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:529" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>19</v>
       </c>
@@ -32466,8 +32520,11 @@
       <c r="TH23" s="8">
         <v>4.4000000000000004</v>
       </c>
+      <c r="TI23" s="8">
+        <v>4.3</v>
+      </c>
     </row>
-    <row r="24" spans="1:528" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:529" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>20</v>
       </c>
@@ -34052,8 +34109,11 @@
       <c r="TH24" s="8">
         <v>4.7</v>
       </c>
+      <c r="TI24" s="8">
+        <v>4.9000000000000004</v>
+      </c>
     </row>
-    <row r="25" spans="1:528" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:529" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
         <v>21</v>
       </c>
@@ -35638,8 +35698,11 @@
       <c r="TH25" s="8">
         <v>2.8</v>
       </c>
+      <c r="TI25" s="8">
+        <v>2.9</v>
+      </c>
     </row>
-    <row r="26" spans="1:528" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:529" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
         <v>22</v>
       </c>
@@ -37224,8 +37287,11 @@
       <c r="TH26" s="8">
         <v>3.6</v>
       </c>
+      <c r="TI26" s="8">
+        <v>3.5</v>
+      </c>
     </row>
-    <row r="27" spans="1:528" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:529" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
         <v>23</v>
       </c>
@@ -38810,8 +38876,11 @@
       <c r="TH27" s="8">
         <v>2.9</v>
       </c>
+      <c r="TI27" s="8">
+        <v>2.8</v>
+      </c>
     </row>
-    <row r="28" spans="1:528" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:529" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
         <v>24</v>
       </c>
@@ -40396,8 +40465,11 @@
       <c r="TH28" s="8">
         <v>4</v>
       </c>
+      <c r="TI28" s="8">
+        <v>3.9</v>
+      </c>
     </row>
-    <row r="29" spans="1:528" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:529" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
         <v>25</v>
       </c>
@@ -41982,8 +42054,11 @@
       <c r="TH29" s="8">
         <v>3.3</v>
       </c>
+      <c r="TI29" s="8">
+        <v>3.3</v>
+      </c>
     </row>
-    <row r="30" spans="1:528" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:529" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
         <v>26</v>
       </c>
@@ -43568,8 +43643,11 @@
       <c r="TH30" s="8">
         <v>5.6</v>
       </c>
+      <c r="TI30" s="8">
+        <v>5.7</v>
+      </c>
     </row>
-    <row r="31" spans="1:528" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:529" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
         <v>27</v>
       </c>
@@ -45154,8 +45232,11 @@
       <c r="TH31" s="8">
         <v>3.1</v>
       </c>
+      <c r="TI31" s="8">
+        <v>3.3</v>
+      </c>
     </row>
-    <row r="32" spans="1:528" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:529" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
         <v>28</v>
       </c>
@@ -46740,8 +46821,11 @@
       <c r="TH32" s="8">
         <v>3.4</v>
       </c>
+      <c r="TI32" s="8">
+        <v>3.4</v>
+      </c>
     </row>
-    <row r="33" spans="1:528" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:529" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
         <v>29</v>
       </c>
@@ -48326,8 +48410,11 @@
       <c r="TH33" s="8">
         <v>3.1</v>
       </c>
+      <c r="TI33" s="8">
+        <v>3.1</v>
+      </c>
     </row>
-    <row r="34" spans="1:528" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:529" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
         <v>30</v>
       </c>
@@ -49912,8 +49999,11 @@
       <c r="TH34" s="8">
         <v>4</v>
       </c>
+      <c r="TI34" s="8">
+        <v>3.8</v>
+      </c>
     </row>
-    <row r="35" spans="1:528" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:529" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
         <v>31</v>
       </c>
@@ -51498,8 +51588,11 @@
       <c r="TH35" s="8">
         <v>2.6</v>
       </c>
+      <c r="TI35" s="8">
+        <v>2.6</v>
+      </c>
     </row>
-    <row r="36" spans="1:528" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:529" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
         <v>32</v>
       </c>
@@ -53084,8 +53177,11 @@
       <c r="TH36" s="8">
         <v>3.4</v>
       </c>
+      <c r="TI36" s="8">
+        <v>3.5</v>
+      </c>
     </row>
-    <row r="37" spans="1:528" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:529" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
         <v>33</v>
       </c>
@@ -54670,8 +54766,11 @@
       <c r="TH37" s="8">
         <v>4.8</v>
       </c>
+      <c r="TI37" s="8">
+        <v>4.7</v>
+      </c>
     </row>
-    <row r="38" spans="1:528" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:529" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
         <v>34</v>
       </c>
@@ -56256,8 +56355,11 @@
       <c r="TH38" s="8">
         <v>4</v>
       </c>
+      <c r="TI38" s="8">
+        <v>4</v>
+      </c>
     </row>
-    <row r="39" spans="1:528" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:529" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
         <v>35</v>
       </c>
@@ -57842,8 +57944,11 @@
       <c r="TH39" s="8">
         <v>3.8</v>
       </c>
+      <c r="TI39" s="8">
+        <v>3.7</v>
+      </c>
     </row>
-    <row r="40" spans="1:528" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:529" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
         <v>36</v>
       </c>
@@ -59428,8 +59533,11 @@
       <c r="TH40" s="8">
         <v>2.5</v>
       </c>
+      <c r="TI40" s="8">
+        <v>2.4</v>
+      </c>
     </row>
-    <row r="41" spans="1:528" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:529" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
         <v>37</v>
       </c>
@@ -61014,8 +61122,11 @@
       <c r="TH41" s="8">
         <v>4.2</v>
       </c>
+      <c r="TI41" s="8">
+        <v>4.2</v>
+      </c>
     </row>
-    <row r="42" spans="1:528" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:529" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
         <v>38</v>
       </c>
@@ -62600,8 +62711,11 @@
       <c r="TH42" s="8">
         <v>3.4</v>
       </c>
+      <c r="TI42" s="8">
+        <v>3.4</v>
+      </c>
     </row>
-    <row r="43" spans="1:528" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:529" x14ac:dyDescent="0.25">
       <c r="A43" s="6" t="s">
         <v>39</v>
       </c>
@@ -64186,8 +64300,11 @@
       <c r="TH43" s="8">
         <v>3.9</v>
       </c>
+      <c r="TI43" s="8">
+        <v>3.7</v>
+      </c>
     </row>
-    <row r="44" spans="1:528" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:529" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
         <v>40</v>
       </c>
@@ -65772,8 +65889,11 @@
       <c r="TH44" s="8">
         <v>4.3</v>
       </c>
+      <c r="TI44" s="8">
+        <v>4.5</v>
+      </c>
     </row>
-    <row r="45" spans="1:528" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:529" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
         <v>41</v>
       </c>
@@ -67358,8 +67478,11 @@
       <c r="TH45" s="8">
         <v>3.5</v>
       </c>
+      <c r="TI45" s="8">
+        <v>3.5</v>
+      </c>
     </row>
-    <row r="46" spans="1:528" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:529" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
         <v>42</v>
       </c>
@@ -68944,8 +69067,11 @@
       <c r="TH46" s="8">
         <v>2.4</v>
       </c>
+      <c r="TI46" s="8">
+        <v>2.2999999999999998</v>
+      </c>
     </row>
-    <row r="47" spans="1:528" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:529" x14ac:dyDescent="0.25">
       <c r="A47" s="6" t="s">
         <v>43</v>
       </c>
@@ -70530,8 +70656,11 @@
       <c r="TH47" s="8">
         <v>3.1</v>
       </c>
+      <c r="TI47" s="8">
+        <v>3.2</v>
+      </c>
     </row>
-    <row r="48" spans="1:528" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:529" x14ac:dyDescent="0.25">
       <c r="A48" s="6" t="s">
         <v>44</v>
       </c>
@@ -72116,8 +72245,11 @@
       <c r="TH48" s="8">
         <v>3.3</v>
       </c>
+      <c r="TI48" s="8">
+        <v>3.3</v>
+      </c>
     </row>
-    <row r="49" spans="1:528" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:529" x14ac:dyDescent="0.25">
       <c r="A49" s="6" t="s">
         <v>45</v>
       </c>
@@ -73702,8 +73834,11 @@
       <c r="TH49" s="8">
         <v>3.4</v>
       </c>
+      <c r="TI49" s="8">
+        <v>3.5</v>
+      </c>
     </row>
-    <row r="50" spans="1:528" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:529" x14ac:dyDescent="0.25">
       <c r="A50" s="6" t="s">
         <v>46</v>
       </c>
@@ -75288,8 +75423,11 @@
       <c r="TH50" s="8">
         <v>2.4</v>
       </c>
+      <c r="TI50" s="8">
+        <v>2.2999999999999998</v>
+      </c>
     </row>
-    <row r="51" spans="1:528" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:529" x14ac:dyDescent="0.25">
       <c r="A51" s="6" t="s">
         <v>47</v>
       </c>
@@ -76874,8 +77012,11 @@
       <c r="TH51" s="8">
         <v>2.2999999999999998</v>
       </c>
+      <c r="TI51" s="8">
+        <v>2.2999999999999998</v>
+      </c>
     </row>
-    <row r="52" spans="1:528" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:529" x14ac:dyDescent="0.25">
       <c r="A52" s="6" t="s">
         <v>48</v>
       </c>
@@ -78460,8 +78601,11 @@
       <c r="TH52" s="8">
         <v>2.6</v>
       </c>
+      <c r="TI52" s="8">
+        <v>2.6</v>
+      </c>
     </row>
-    <row r="53" spans="1:528" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:529" x14ac:dyDescent="0.25">
       <c r="A53" s="6" t="s">
         <v>49</v>
       </c>
@@ -80046,8 +80190,11 @@
       <c r="TH53" s="8">
         <v>4.4000000000000004</v>
       </c>
+      <c r="TI53" s="8">
+        <v>4.3</v>
+      </c>
     </row>
-    <row r="54" spans="1:528" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:529" x14ac:dyDescent="0.25">
       <c r="A54" s="6" t="s">
         <v>50</v>
       </c>
@@ -81632,8 +81779,11 @@
       <c r="TH54" s="8">
         <v>4.9000000000000004</v>
       </c>
+      <c r="TI54" s="8">
+        <v>5</v>
+      </c>
     </row>
-    <row r="55" spans="1:528" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:529" x14ac:dyDescent="0.25">
       <c r="A55" s="6" t="s">
         <v>51</v>
       </c>
@@ -83218,8 +83368,11 @@
       <c r="TH55" s="8">
         <v>3.3</v>
       </c>
+      <c r="TI55" s="8">
+        <v>3.4</v>
+      </c>
     </row>
-    <row r="56" spans="1:528" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:529" x14ac:dyDescent="0.25">
       <c r="A56" s="6" t="s">
         <v>52</v>
       </c>
@@ -84802,6 +84955,9 @@
         <v>3.8</v>
       </c>
       <c r="TH56" s="8">
+        <v>3.7</v>
+      </c>
+      <c r="TI56" s="8">
         <v>3.7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
SEM update on Jan. 24th, 2023
</commit_message>
<xml_diff>
--- a/static/data/source/unemployment_rate.xlsx
+++ b/static/data/source/unemployment_rate.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="616" uniqueCount="616">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="617" uniqueCount="617">
   <si>
     <t xml:space="preserve">Geography</t>
   </si>
@@ -1706,6 +1706,9 @@
     <t xml:space="preserve">11/01/2022</t>
   </si>
   <si>
+    <t xml:space="preserve">12/01/2022</t>
+  </si>
+  <si>
     <t xml:space="preserve">United States</t>
   </si>
   <si>
@@ -3884,10 +3887,13 @@
       <c r="UR4" t="s">
         <v>563</v>
       </c>
+      <c r="US4" t="s">
+        <v>564</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="B5" t="n">
         <v>7.9</v>
@@ -5450,7 +5456,7 @@
         <v>3.6</v>
       </c>
       <c r="TB5" t="n">
-        <v>3.6</v>
+        <v>3.7</v>
       </c>
       <c r="TC5" t="n">
         <v>3.6</v>
@@ -5510,16 +5516,16 @@
         <v>6.7</v>
       </c>
       <c r="TV5" t="n">
-        <v>6.4</v>
+        <v>6.3</v>
       </c>
       <c r="TW5" t="n">
         <v>6.2</v>
       </c>
       <c r="TX5" t="n">
-        <v>6</v>
+        <v>6.1</v>
       </c>
       <c r="TY5" t="n">
-        <v>6</v>
+        <v>6.1</v>
       </c>
       <c r="TZ5" t="n">
         <v>5.8</v>
@@ -5534,10 +5540,10 @@
         <v>5.2</v>
       </c>
       <c r="UD5" t="n">
-        <v>4.7</v>
+        <v>4.8</v>
       </c>
       <c r="UE5" t="n">
-        <v>4.6</v>
+        <v>4.5</v>
       </c>
       <c r="UF5" t="n">
         <v>4.2</v>
@@ -5576,12 +5582,15 @@
         <v>3.7</v>
       </c>
       <c r="UR5" t="n">
-        <v>3.7</v>
+        <v>3.6</v>
+      </c>
+      <c r="US5" t="n">
+        <v>3.5</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
       <c r="B6" t="n">
         <v>6.6</v>
@@ -7271,11 +7280,14 @@
       </c>
       <c r="UR6" t="n">
         <v>2.7</v>
+      </c>
+      <c r="US6" t="n">
+        <v>2.8</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="B7" t="n">
         <v>7.1</v>
@@ -8965,11 +8977,14 @@
       </c>
       <c r="UR7" t="n">
         <v>4.5</v>
+      </c>
+      <c r="US7" t="n">
+        <v>4.3</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="B8" t="n">
         <v>10.2</v>
@@ -10659,11 +10674,14 @@
       </c>
       <c r="UR8" t="n">
         <v>4.1</v>
+      </c>
+      <c r="US8" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="B9" t="n">
         <v>7.3</v>
@@ -12353,11 +12371,14 @@
       </c>
       <c r="UR9" t="n">
         <v>3.7</v>
+      </c>
+      <c r="US9" t="n">
+        <v>3.6</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="B10" t="n">
         <v>9.2</v>
@@ -14046,12 +14067,15 @@
         <v>4</v>
       </c>
       <c r="UR10" t="n">
+        <v>4.1</v>
+      </c>
+      <c r="US10" t="n">
         <v>4.1</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
       <c r="B11" t="n">
         <v>5.8</v>
@@ -15741,11 +15765,14 @@
       </c>
       <c r="UR11" t="n">
         <v>3.5</v>
+      </c>
+      <c r="US11" t="n">
+        <v>3.3</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="B12" t="n">
         <v>9.8</v>
@@ -17434,12 +17461,15 @@
         <v>4.3</v>
       </c>
       <c r="UR12" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="US12" t="n">
         <v>4.2</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
       <c r="B13" t="n">
         <v>8</v>
@@ -19128,12 +19158,15 @@
         <v>4.3</v>
       </c>
       <c r="UR13" t="n">
+        <v>4.4</v>
+      </c>
+      <c r="US13" t="n">
         <v>4.4</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>573</v>
+        <v>574</v>
       </c>
       <c r="B14" t="n">
         <v>8.7</v>
@@ -20823,11 +20856,14 @@
       </c>
       <c r="UR14" t="n">
         <v>4.6</v>
+      </c>
+      <c r="US14" t="n">
+        <v>4.7</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
       <c r="B15" t="n">
         <v>9.7</v>
@@ -22517,11 +22553,14 @@
       </c>
       <c r="UR15" t="n">
         <v>2.6</v>
+      </c>
+      <c r="US15" t="n">
+        <v>2.5</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
       <c r="B16" t="n">
         <v>8.4</v>
@@ -24210,12 +24249,15 @@
         <v>2.9</v>
       </c>
       <c r="UR16" t="n">
+        <v>3</v>
+      </c>
+      <c r="US16" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
       <c r="B17" t="n">
         <v>9.8</v>
@@ -25905,11 +25947,14 @@
       </c>
       <c r="UR17" t="n">
         <v>3.3</v>
+      </c>
+      <c r="US17" t="n">
+        <v>3.2</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
       <c r="B18" t="n">
         <v>5.6</v>
@@ -27599,11 +27644,14 @@
       </c>
       <c r="UR18" t="n">
         <v>3</v>
+      </c>
+      <c r="US18" t="n">
+        <v>2.9</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
       <c r="B19" t="n">
         <v>6.6</v>
@@ -29292,12 +29340,15 @@
         <v>4.6</v>
       </c>
       <c r="UR19" t="n">
+        <v>4.7</v>
+      </c>
+      <c r="US19" t="n">
         <v>4.7</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="B20" t="n">
         <v>6.6</v>
@@ -30987,11 +31038,14 @@
       </c>
       <c r="UR20" t="n">
         <v>3</v>
+      </c>
+      <c r="US20" t="n">
+        <v>3.1</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
       <c r="B21" t="n">
         <v>4.3</v>
@@ -32680,12 +32734,15 @@
         <v>2.9</v>
       </c>
       <c r="UR21" t="n">
+        <v>3.1</v>
+      </c>
+      <c r="US21" t="n">
         <v>3.1</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="B22" t="n">
         <v>4.2</v>
@@ -34375,11 +34432,14 @@
       </c>
       <c r="UR22" t="n">
         <v>2.8</v>
+      </c>
+      <c r="US22" t="n">
+        <v>2.9</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>582</v>
+        <v>583</v>
       </c>
       <c r="B23" t="n">
         <v>5.6</v>
@@ -36068,12 +36128,15 @@
         <v>3.9</v>
       </c>
       <c r="UR23" t="n">
+        <v>4</v>
+      </c>
+      <c r="US23" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="B24" t="n">
         <v>6.3</v>
@@ -37763,11 +37826,14 @@
       </c>
       <c r="UR24" t="n">
         <v>3.3</v>
+      </c>
+      <c r="US24" t="n">
+        <v>3.5</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>584</v>
+        <v>585</v>
       </c>
       <c r="B25" t="n">
         <v>8.7</v>
@@ -39457,11 +39523,14 @@
       </c>
       <c r="UR25" t="n">
         <v>3.7</v>
+      </c>
+      <c r="US25" t="n">
+        <v>3.8</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
       <c r="B26" t="n">
         <v>6.4</v>
@@ -41151,11 +41220,14 @@
       </c>
       <c r="UR26" t="n">
         <v>4.3</v>
+      </c>
+      <c r="US26" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
       <c r="B27" t="n">
         <v>10.5</v>
@@ -42845,11 +42917,14 @@
       </c>
       <c r="UR27" t="n">
         <v>3.4</v>
+      </c>
+      <c r="US27" t="n">
+        <v>3.3</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>587</v>
+        <v>588</v>
       </c>
       <c r="B28" t="n">
         <v>9.9</v>
@@ -44538,12 +44613,15 @@
         <v>4.2</v>
       </c>
       <c r="UR28" t="n">
+        <v>4.3</v>
+      </c>
+      <c r="US28" t="n">
         <v>4.3</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
       <c r="B29" t="n">
         <v>6</v>
@@ -46233,11 +46311,14 @@
       </c>
       <c r="UR29" t="n">
         <v>2.3</v>
+      </c>
+      <c r="US29" t="n">
+        <v>2.5</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="B30" t="n">
         <v>6.7</v>
@@ -47927,11 +48008,14 @@
       </c>
       <c r="UR30" t="n">
         <v>3.9</v>
+      </c>
+      <c r="US30" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
       <c r="B31" t="n">
         <v>5.9</v>
@@ -49621,11 +49705,14 @@
       </c>
       <c r="UR31" t="n">
         <v>2.7</v>
+      </c>
+      <c r="US31" t="n">
+        <v>2.8</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>591</v>
+        <v>592</v>
       </c>
       <c r="B32" t="n">
         <v>5.8</v>
@@ -51315,11 +51402,14 @@
       </c>
       <c r="UR32" t="n">
         <v>2.9</v>
+      </c>
+      <c r="US32" t="n">
+        <v>2.8</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
       <c r="B33" t="n">
         <v>3.3</v>
@@ -53009,11 +53099,14 @@
       </c>
       <c r="UR33" t="n">
         <v>2.5</v>
+      </c>
+      <c r="US33" t="n">
+        <v>2.6</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
       <c r="B34" t="n">
         <v>9.2</v>
@@ -54703,11 +54796,14 @@
       </c>
       <c r="UR34" t="n">
         <v>4.9</v>
+      </c>
+      <c r="US34" t="n">
+        <v>5.2</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>594</v>
+        <v>595</v>
       </c>
       <c r="B35" t="n">
         <v>6.5</v>
@@ -56397,11 +56493,14 @@
       </c>
       <c r="UR35" t="n">
         <v>2.6</v>
+      </c>
+      <c r="US35" t="n">
+        <v>2.7</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
       <c r="B36" t="n">
         <v>10.3</v>
@@ -58090,12 +58189,15 @@
         <v>3.4</v>
       </c>
       <c r="UR36" t="n">
+        <v>3.4</v>
+      </c>
+      <c r="US36" t="n">
         <v>3.4</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>596</v>
+        <v>597</v>
       </c>
       <c r="B37" t="n">
         <v>8.6</v>
@@ -59785,11 +59887,14 @@
       </c>
       <c r="UR37" t="n">
         <v>4.1</v>
+      </c>
+      <c r="US37" t="n">
+        <v>3.9</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>597</v>
+        <v>598</v>
       </c>
       <c r="B38" t="n">
         <v>10.3</v>
@@ -61478,12 +61583,15 @@
         <v>4.3</v>
       </c>
       <c r="UR38" t="n">
+        <v>4.3</v>
+      </c>
+      <c r="US38" t="n">
         <v>4.3</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>598</v>
+        <v>599</v>
       </c>
       <c r="B39" t="n">
         <v>6.4</v>
@@ -63172,12 +63280,15 @@
         <v>3.8</v>
       </c>
       <c r="UR39" t="n">
+        <v>3.9</v>
+      </c>
+      <c r="US39" t="n">
         <v>3.9</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>599</v>
+        <v>600</v>
       </c>
       <c r="B40" t="n">
         <v>3.4</v>
@@ -64866,12 +64977,15 @@
         <v>2.3</v>
       </c>
       <c r="UR40" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="US40" t="n">
         <v>2.3</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>600</v>
+        <v>601</v>
       </c>
       <c r="B41" t="n">
         <v>8.1</v>
@@ -66560,12 +66674,15 @@
         <v>4.2</v>
       </c>
       <c r="UR41" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="US41" t="n">
         <v>4.2</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>601</v>
+        <v>602</v>
       </c>
       <c r="B42" t="n">
         <v>5.8</v>
@@ -68254,12 +68371,15 @@
         <v>3.4</v>
       </c>
       <c r="UR42" t="n">
+        <v>3.4</v>
+      </c>
+      <c r="US42" t="n">
         <v>3.4</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>602</v>
+        <v>603</v>
       </c>
       <c r="B43" t="n">
         <v>9.5</v>
@@ -69948,12 +70068,15 @@
         <v>4.1</v>
       </c>
       <c r="UR43" t="n">
-        <v>4.4</v>
+        <v>4.3</v>
+      </c>
+      <c r="US43" t="n">
+        <v>4.5</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="B44" t="n">
         <v>8</v>
@@ -71643,11 +71766,14 @@
       </c>
       <c r="UR44" t="n">
         <v>4</v>
+      </c>
+      <c r="US44" t="n">
+        <v>3.9</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>604</v>
+        <v>605</v>
       </c>
       <c r="B45" t="n">
         <v>7.8</v>
@@ -73337,11 +73463,14 @@
       </c>
       <c r="UR45" t="n">
         <v>3.6</v>
+      </c>
+      <c r="US45" t="n">
+        <v>3.5</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
       <c r="B46" t="n">
         <v>7.4</v>
@@ -75030,12 +75159,15 @@
         <v>3.3</v>
       </c>
       <c r="UR46" t="n">
+        <v>3.3</v>
+      </c>
+      <c r="US46" t="n">
         <v>3.3</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="B47" t="n">
         <v>3.3</v>
@@ -76725,11 +76857,14 @@
       </c>
       <c r="UR47" t="n">
         <v>2.4</v>
+      </c>
+      <c r="US47" t="n">
+        <v>2.3</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
       <c r="B48" t="n">
         <v>6</v>
@@ -78418,12 +78553,15 @@
         <v>3.5</v>
       </c>
       <c r="UR48" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="US48" t="n">
         <v>3.5</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
       <c r="B49" t="n">
         <v>5.8</v>
@@ -80113,11 +80251,14 @@
       </c>
       <c r="UR49" t="n">
         <v>4</v>
+      </c>
+      <c r="US49" t="n">
+        <v>3.9</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="B50" t="n">
         <v>5.8</v>
@@ -81806,12 +81947,15 @@
         <v>2.1</v>
       </c>
       <c r="UR50" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="US50" t="n">
         <v>2.2</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="B51" t="n">
         <v>8.6</v>
@@ -83501,11 +83645,14 @@
       </c>
       <c r="UR51" t="n">
         <v>2.5</v>
+      </c>
+      <c r="US51" t="n">
+        <v>2.6</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>611</v>
+        <v>612</v>
       </c>
       <c r="B52" t="n">
         <v>6.1</v>
@@ -85195,11 +85342,14 @@
       </c>
       <c r="UR52" t="n">
         <v>2.8</v>
+      </c>
+      <c r="US52" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
       <c r="B53" t="n">
         <v>8.5</v>
@@ -86889,11 +87039,14 @@
       </c>
       <c r="UR53" t="n">
         <v>4</v>
+      </c>
+      <c r="US53" t="n">
+        <v>4.2</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="B54" t="n">
         <v>7.5</v>
@@ -88582,12 +88735,15 @@
         <v>4</v>
       </c>
       <c r="UR54" t="n">
+        <v>4.1</v>
+      </c>
+      <c r="US54" t="n">
         <v>4.1</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="B55" t="n">
         <v>5.8</v>
@@ -90277,11 +90433,14 @@
       </c>
       <c r="UR55" t="n">
         <v>3.3</v>
+      </c>
+      <c r="US55" t="n">
+        <v>3.2</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
       <c r="B56" t="n">
         <v>4.1</v>
@@ -91971,6 +92130,9 @@
       </c>
       <c r="UR56" t="n">
         <v>3.6</v>
+      </c>
+      <c r="US56" t="n">
+        <v>3.7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>